<commit_message>
update prompt for Assistant
</commit_message>
<xml_diff>
--- a/runtime/apps/conneXion/conneXion.xlsx
+++ b/runtime/apps/conneXion/conneXion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\runtime\apps\conneXion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DFB38C-5DCB-4192-A5D0-173D91E5C276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D3E99D-4FD7-4884-B222-DCF364F50E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" firstSheet="2" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="162">
   <si>
     <t>Parameter</t>
   </si>
@@ -132,9 +132,6 @@
     <t>body_fr</t>
   </si>
   <si>
-    <t>Expiration de votre API</t>
-  </si>
-  <si>
     <t>subject_fr</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>CONTEXT</t>
   </si>
   <si>
-    <t>USER</t>
-  </si>
-  <si>
     <t>smtp_server</t>
   </si>
   <si>
@@ -186,29 +180,6 @@
     <t>distribution_engine</t>
   </si>
   <si>
-    <t>{prenom} {nom},
-Nous avons traité votre demande du {date_demande} en rapport avec l'expiration d'une API</t>
-  </si>
-  <si>
-    <t>api-a-renouveler</t>
-  </si>
-  <si>
-    <t>sauf-conduits</t>
-  </si>
-  <si>
-    <t>Votre demande de sauf-conduit</t>
-  </si>
-  <si>
-    <t>{prenom} {nom},
-En réponse à votre demande, je vous invite à nous adresser une copie des éléments suivants :
-- l’acte de décès traduit
-- votre acte de naissance
-- la date des funérailles
-- votre carte de séjour
-- d'un justificatif de domicile de moins de 6 mois en indiquant en objet URGENT DEMANDE DE SAUF CONDUIT.
-En espérant vous avoir apporté les éléments souhaités,</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -290,26 +261,6 @@
     <t>Document de Circulation pour Etranger Mineur (Travel Document for a Minor Foreigner)</t>
   </si>
   <si>
-    <t>Expiration of your API</t>
-  </si>
-  <si>
-    <t>{prenom} {nom},
-We have processed your request dated {date_demande} regarding the expiration of an API</t>
-  </si>
-  <si>
-    <t>Your request for a safe‑conduct pass</t>
-  </si>
-  <si>
-    <t>{prenom} {nom},
-In response to your request, please send us copies of the following:
-the translated death certificate
-your birth certificate
-the date of the funeral
-your residence permit
-proof of address less than six months old, with “URGENT REQUEST FOR A SAFE-CONDUCT” in the subject line.
-I hope this gives you the information you were looking for.</t>
-  </si>
-  <si>
     <t>app_name_en</t>
   </si>
   <si>
@@ -356,9 +307,6 @@
   </si>
   <si>
     <t>Attestation de Demande d’Asile (Certificate of Asylum Application)</t>
-  </si>
-  <si>
-    <t>Ready to copy-paste values</t>
   </si>
   <si>
     <t>True</t>
@@ -580,9 +528,6 @@
     <t>do not rename as it is the default value for v1 legacy calls</t>
   </si>
   <si>
-    <t>preprocessing</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -592,7 +537,13 @@
     <t>DecisionEngineConnexion</t>
   </si>
   <si>
-    <t>runtime.apps.conneXion.preprocessing.preprocessing</t>
+    <t>data_enrichment</t>
+  </si>
+  <si>
+    <t>runtime.apps.conneXion.data_enrichment.data_enrichment</t>
+  </si>
+  <si>
+    <t>REQUESTER</t>
   </si>
 </sst>
 </file>
@@ -683,7 +634,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -719,12 +670,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1041,12 +986,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1059,65 +1004,65 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1121,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,39 +1138,39 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1277,25 +1222,25 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
@@ -1304,25 +1249,25 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="5">
         <v>587</v>
@@ -1331,13 +1276,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1352,11 +1297,9 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1371,50 +1314,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +1338,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
@@ -1457,7 +1366,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1465,100 +1374,100 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1571,7 +1480,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,19 +1503,19 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -1643,37 +1552,37 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -1699,26 +1608,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1744,42 +1653,42 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1791,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,7 +1714,7 @@
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.42578125" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
     <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="77" bestFit="1" customWidth="1"/>
@@ -1818,28 +1727,28 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>22</v>
@@ -1848,7 +1757,7 @@
         <v>17</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>18</v>
@@ -1859,354 +1768,354 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>169</v>
-      </c>
       <c r="I9" s="8" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2237,10 +2146,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,15 +2157,10 @@
     <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="86.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="59.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2266,54 +2170,27 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-    </row>
-    <row r="2" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-    </row>
-    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:N1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2339,7 +2216,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>14</v>
@@ -2350,10 +2227,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2361,7 +2238,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
@@ -2372,10 +2249,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2383,10 +2260,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2394,10 +2271,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>